<commit_message>
sửa lại template file excel bảng mapping
</commit_message>
<xml_diff>
--- a/public/excel/Mapping.xlsx
+++ b/public/excel/Mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TLG\DeliveryTracking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soft.public\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
-  <si>
-    <t>Mã Map</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>SKUS-KH</t>
   </si>
@@ -56,18 +53,6 @@
     <t>Tỷ lệ màu</t>
   </si>
   <si>
-    <t>Winmart</t>
-  </si>
-  <si>
-    <t>10316863</t>
-  </si>
-  <si>
-    <t>TL Vỉ 2 Gôm E-017/FR</t>
-  </si>
-  <si>
-    <t>VI</t>
-  </si>
-  <si>
     <t>50007177</t>
   </si>
   <si>
@@ -77,40 +62,13 @@
     <t>SET</t>
   </si>
   <si>
-    <t>10315837</t>
-  </si>
-  <si>
-    <t>TL Bộ sáp nặn MCT - C01/DO - 16 món</t>
-  </si>
-  <si>
-    <t>ZBO</t>
-  </si>
-  <si>
-    <t>50005343</t>
-  </si>
-  <si>
-    <t>Bộ sáp nặn MCT-C01/DO hộp 16</t>
-  </si>
-  <si>
-    <t>CAN</t>
-  </si>
-  <si>
-    <t>10280962</t>
-  </si>
-  <si>
-    <t>TL Kéo văn phòng SC-016 hộp 20/T240</t>
-  </si>
-  <si>
     <t>CAI</t>
   </si>
   <si>
-    <t>50008514</t>
-  </si>
-  <si>
-    <t>Kéo văn phòng SC-016 hộp 20/T240</t>
-  </si>
-  <si>
-    <t>PC</t>
+    <t>Nhóm KH</t>
+  </si>
+  <si>
+    <t>Emart</t>
   </si>
 </sst>
 </file>
@@ -453,139 +411,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>8936040451101</v>
+      </c>
+      <c r="C2">
+        <v>8936040451101</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="J2" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="2">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sửa dữ liệu template excel bảng mapping
</commit_message>
<xml_diff>
--- a/public/excel/Mapping.xlsx
+++ b/public/excel/Mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\soft.public\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TLG\DeliveryTracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -75,7 +75,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +87,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -127,10 +142,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,7 +431,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,11 +450,11 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -465,11 +482,11 @@
       <c r="C2">
         <v>8936040451101</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>9</v>

</xml_diff>